<commit_message>
Re-ran solver, got the correct solution that matches graphical method
</commit_message>
<xml_diff>
--- a/optimisation/hw/hw1/q1_solve.xlsx
+++ b/optimisation/hw/hw1/q1_solve.xlsx
@@ -4,56 +4,58 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sensitivity Report 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Sensitivity Report 2" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$9:$C$9</definedName>
-    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$16</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$B$17</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$B$18</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$B$19</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Sheet1!$B$20</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">Sheet1!$B$21</definedName>
-    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">6</definedName>
-    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$B$12</definedName>
-    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
-    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$C$16</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$C$17</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$C$18</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$C$19</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Sheet1!$C$20</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">Sheet1!$C$21</definedName>
-    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_tim" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">Sheet1!$B$9:$C$9</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">Sheet1!$B$16</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">Sheet1!$B$17</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">Sheet1!$B$18</definedName>
+    <definedName name="solver_lhs4" localSheetId="2" hidden="1">Sheet1!$B$19</definedName>
+    <definedName name="solver_lhs5" localSheetId="2" hidden="1">Sheet1!$B$20</definedName>
+    <definedName name="solver_lhs6" localSheetId="2" hidden="1">Sheet1!$B$21</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">6</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">Sheet1!$B$12</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">Sheet1!$C$16</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">Sheet1!$C$17</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">Sheet1!$C$18</definedName>
+    <definedName name="solver_rhs4" localSheetId="2" hidden="1">Sheet1!$C$19</definedName>
+    <definedName name="solver_rhs5" localSheetId="2" hidden="1">Sheet1!$C$20</definedName>
+    <definedName name="solver_rhs6" localSheetId="2" hidden="1">Sheet1!$C$21</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">100</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.05</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="59">
   <si>
     <t>Work-hours per unit</t>
   </si>
@@ -113,13 +115,130 @@
   </si>
   <si>
     <t>Non-neg 2</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 12.0 Sensitivity Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [q1_solve.xlsx]Sheet1</t>
+  </si>
+  <si>
+    <t>Report Created: 26/11/2015 13:24:37</t>
+  </si>
+  <si>
+    <t>Adjustable Cells</t>
+  </si>
+  <si>
+    <t>Cell</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Lagrange</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>$B$9</t>
+  </si>
+  <si>
+    <t>Quota F</t>
+  </si>
+  <si>
+    <t>$C$9</t>
+  </si>
+  <si>
+    <t>Quota C</t>
+  </si>
+  <si>
+    <t>$B$16</t>
+  </si>
+  <si>
+    <t>GA LHS</t>
+  </si>
+  <si>
+    <t>$B$17</t>
+  </si>
+  <si>
+    <t>Elect LHS</t>
+  </si>
+  <si>
+    <t>$B$18</t>
+  </si>
+  <si>
+    <t>Demand F LHS</t>
+  </si>
+  <si>
+    <t>$B$19</t>
+  </si>
+  <si>
+    <t>Demand C LHS</t>
+  </si>
+  <si>
+    <t>$B$20</t>
+  </si>
+  <si>
+    <t>Non-neg 1 LHS</t>
+  </si>
+  <si>
+    <t>$B$21</t>
+  </si>
+  <si>
+    <t>Non-neg 2 LHS</t>
+  </si>
+  <si>
+    <t>Report Created: 26/11/2015 13:25:33</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Allowable</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
+  <si>
+    <t>Decrease</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>R.H. Side</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -150,6 +269,21 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -165,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -188,15 +322,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -204,6 +373,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -566,11 +749,535 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="14">
+        <v>175</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="15">
+        <v>150</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1">
+      <c r="B14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="14">
+        <v>500</v>
+      </c>
+      <c r="E15" s="14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="14">
+        <v>800</v>
+      </c>
+      <c r="E16" s="14">
+        <v>34.999999999999986</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="14">
+        <v>175</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="14">
+        <v>150</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="14">
+        <v>175</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="15">
+        <v>150</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="14">
+        <v>175</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>120</v>
+      </c>
+      <c r="G9" s="10">
+        <v>140</v>
+      </c>
+      <c r="H9" s="10">
+        <v>33.333333333333336</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="15">
+        <v>150</v>
+      </c>
+      <c r="E10" s="15">
+        <v>0</v>
+      </c>
+      <c r="F10" s="11">
+        <v>130</v>
+      </c>
+      <c r="G10" s="11">
+        <v>50</v>
+      </c>
+      <c r="H10" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1">
+      <c r="B14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="14">
+        <v>500</v>
+      </c>
+      <c r="E15" s="14">
+        <v>25</v>
+      </c>
+      <c r="F15" s="10">
+        <v>500</v>
+      </c>
+      <c r="G15" s="10">
+        <v>60</v>
+      </c>
+      <c r="H15" s="10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="14">
+        <v>800</v>
+      </c>
+      <c r="E16" s="14">
+        <v>35</v>
+      </c>
+      <c r="F16" s="10">
+        <v>800</v>
+      </c>
+      <c r="G16" s="10">
+        <v>60</v>
+      </c>
+      <c r="H16" s="10">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="14">
+        <v>175</v>
+      </c>
+      <c r="E17" s="14">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>220</v>
+      </c>
+      <c r="G17" s="10">
+        <v>1E+30</v>
+      </c>
+      <c r="H17" s="10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="14">
+        <v>150</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>180</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1E+30</v>
+      </c>
+      <c r="H18" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="14">
+        <v>175</v>
+      </c>
+      <c r="E19" s="14">
+        <v>0</v>
+      </c>
+      <c r="F19" s="10">
+        <v>0</v>
+      </c>
+      <c r="G19" s="10">
+        <v>175</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B20" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="15">
+        <v>150</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>150</v>
+      </c>
+      <c r="H20" s="11">
+        <v>1E+30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -582,55 +1289,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>500</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>800</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -641,46 +1348,46 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>120</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3">
-        <v>130</v>
-      </c>
-      <c r="C9" s="3">
-        <v>180</v>
+      <c r="B9" s="2">
+        <v>175</v>
+      </c>
+      <c r="C9" s="2">
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12">
         <f>B9*B6+C9*C6</f>
-        <v>39000</v>
+        <v>40500</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -701,7 +1408,7 @@
       </c>
       <c r="B16">
         <f>B3*B9+C3*C9</f>
-        <v>440</v>
+        <v>500</v>
       </c>
       <c r="C16">
         <f>D3</f>
@@ -727,7 +1434,7 @@
       </c>
       <c r="B18">
         <f>B9</f>
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="C18">
         <f>B5</f>
@@ -740,7 +1447,7 @@
       </c>
       <c r="B19">
         <f>C9</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C19">
         <f>C5</f>
@@ -753,7 +1460,7 @@
       </c>
       <c r="B20">
         <f>B9</f>
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -765,7 +1472,7 @@
       </c>
       <c r="B21">
         <f>C9</f>
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -780,7 +1487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
@@ -796,7 +1503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>